<commit_message>
this can auto detect best 5 jet imgs
</commit_message>
<xml_diff>
--- a/profile.xlsx
+++ b/profile.xlsx
@@ -332,10 +332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,6 +623,289 @@
         <v>981</v>
       </c>
     </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20200107</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>-961</v>
+      </c>
+      <c r="L9">
+        <v>1282.28</v>
+      </c>
+      <c r="M9">
+        <v>858.35</v>
+      </c>
+      <c r="N9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20200107</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>-960</v>
+      </c>
+      <c r="L10">
+        <v>1282.9100000000001</v>
+      </c>
+      <c r="M10">
+        <v>937.86</v>
+      </c>
+      <c r="N10">
+        <v>45.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20200107</v>
+      </c>
+      <c r="B11">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>-959</v>
+      </c>
+      <c r="L11">
+        <v>1282.0999999999999</v>
+      </c>
+      <c r="M11">
+        <v>1018.4</v>
+      </c>
+      <c r="N11">
+        <v>44.41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>20200107</v>
+      </c>
+      <c r="B12">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2020</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>17</v>
+      </c>
+      <c r="I12">
+        <v>21</v>
+      </c>
+      <c r="J12" s="1">
+        <v>9.94</v>
+      </c>
+      <c r="K12">
+        <v>-911</v>
+      </c>
+      <c r="L12">
+        <v>1285</v>
+      </c>
+      <c r="M12">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20200107</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>2020</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>17</v>
+      </c>
+      <c r="I13">
+        <v>21</v>
+      </c>
+      <c r="J13" s="1">
+        <v>9.94</v>
+      </c>
+      <c r="K13">
+        <v>-910</v>
+      </c>
+      <c r="L13">
+        <v>1265</v>
+      </c>
+      <c r="M13">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20200107</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>2020</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>17</v>
+      </c>
+      <c r="I14">
+        <v>21</v>
+      </c>
+      <c r="J14" s="1">
+        <v>9.94</v>
+      </c>
+      <c r="K14">
+        <v>-909</v>
+      </c>
+      <c r="L14">
+        <v>1261</v>
+      </c>
+      <c r="M14">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20200107</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>2020</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>17</v>
+      </c>
+      <c r="I15">
+        <v>21</v>
+      </c>
+      <c r="J15" s="1">
+        <v>9.94</v>
+      </c>
+      <c r="K15">
+        <v>-908</v>
+      </c>
+      <c r="L15">
+        <v>1290</v>
+      </c>
+      <c r="M15">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>20200107</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2020</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>17</v>
+      </c>
+      <c r="I16">
+        <v>21</v>
+      </c>
+      <c r="J16" s="1">
+        <v>9.94</v>
+      </c>
+      <c r="K16">
+        <v>-907</v>
+      </c>
+      <c r="L16">
+        <v>1282</v>
+      </c>
+      <c r="M16">
+        <v>982</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
this works well untill 14 6 1
</commit_message>
<xml_diff>
--- a/profile.xlsx
+++ b/profile.xlsx
@@ -332,10 +332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,6 +906,289 @@
         <v>982</v>
       </c>
     </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20200107</v>
+      </c>
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>-1055</v>
+      </c>
+      <c r="L17">
+        <v>1283.82</v>
+      </c>
+      <c r="M17">
+        <v>841.79</v>
+      </c>
+      <c r="N17">
+        <v>45.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20200107</v>
+      </c>
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>-1054</v>
+      </c>
+      <c r="L18">
+        <v>1285.23</v>
+      </c>
+      <c r="M18">
+        <v>921.77</v>
+      </c>
+      <c r="N18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20200107</v>
+      </c>
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>-1053</v>
+      </c>
+      <c r="L19">
+        <v>1284.5</v>
+      </c>
+      <c r="M19">
+        <v>1001.86</v>
+      </c>
+      <c r="N19">
+        <v>45.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20200107</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>2020</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
+      <c r="I20">
+        <v>14</v>
+      </c>
+      <c r="J20" s="1">
+        <v>49.561999999999998</v>
+      </c>
+      <c r="K20">
+        <v>-1002</v>
+      </c>
+      <c r="L20">
+        <v>1280</v>
+      </c>
+      <c r="M20">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20200107</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>2020</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>18</v>
+      </c>
+      <c r="I21">
+        <v>14</v>
+      </c>
+      <c r="J21" s="1">
+        <v>49.561999999999998</v>
+      </c>
+      <c r="K21">
+        <v>-1001</v>
+      </c>
+      <c r="L21">
+        <v>1280</v>
+      </c>
+      <c r="M21">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20200107</v>
+      </c>
+      <c r="B22">
+        <v>14</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>2020</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>18</v>
+      </c>
+      <c r="I22">
+        <v>14</v>
+      </c>
+      <c r="J22" s="1">
+        <v>49.561999999999998</v>
+      </c>
+      <c r="K22">
+        <v>-1000</v>
+      </c>
+      <c r="L22">
+        <v>1280</v>
+      </c>
+      <c r="M22">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20200107</v>
+      </c>
+      <c r="B23">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>2020</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>18</v>
+      </c>
+      <c r="I23">
+        <v>14</v>
+      </c>
+      <c r="J23" s="1">
+        <v>49.561999999999998</v>
+      </c>
+      <c r="K23">
+        <v>-999</v>
+      </c>
+      <c r="L23">
+        <v>1283</v>
+      </c>
+      <c r="M23">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20200107</v>
+      </c>
+      <c r="B24">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>2020</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>10</v>
+      </c>
+      <c r="H24">
+        <v>18</v>
+      </c>
+      <c r="I24">
+        <v>14</v>
+      </c>
+      <c r="J24" s="1">
+        <v>49.561999999999998</v>
+      </c>
+      <c r="K24">
+        <v>-998</v>
+      </c>
+      <c r="L24">
+        <v>1284</v>
+      </c>
+      <c r="M24">
+        <v>922</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
from 0107 to 0108, modify the entension name
</commit_message>
<xml_diff>
--- a/profile.xlsx
+++ b/profile.xlsx
@@ -332,10 +332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection sqref="A1:N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1189,372 @@
         <v>922</v>
       </c>
     </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20200107</v>
+      </c>
+      <c r="B25">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25">
+        <v>-798</v>
+      </c>
+      <c r="L25">
+        <v>1277.19</v>
+      </c>
+      <c r="M25">
+        <v>890.06</v>
+      </c>
+      <c r="N25">
+        <v>47.12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>20200107</v>
+      </c>
+      <c r="B26">
+        <v>14</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26">
+        <v>-797</v>
+      </c>
+      <c r="L26">
+        <v>1278.25</v>
+      </c>
+      <c r="M26">
+        <v>946.21</v>
+      </c>
+      <c r="N26">
+        <v>46.19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>20200107</v>
+      </c>
+      <c r="B27">
+        <v>14</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27">
+        <v>-796</v>
+      </c>
+      <c r="L27">
+        <v>1278.31</v>
+      </c>
+      <c r="M27">
+        <v>1002.32</v>
+      </c>
+      <c r="N27">
+        <v>45.74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>20200107</v>
+      </c>
+      <c r="B28">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>2020</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <v>18</v>
+      </c>
+      <c r="I28">
+        <v>19</v>
+      </c>
+      <c r="J28" s="1">
+        <v>41.476999999999997</v>
+      </c>
+      <c r="K28">
+        <v>-754</v>
+      </c>
+      <c r="L28" s="1">
+        <v>254.16</v>
+      </c>
+      <c r="M28">
+        <v>957.22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>20200107</v>
+      </c>
+      <c r="B29">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>2020</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="H29">
+        <v>18</v>
+      </c>
+      <c r="I29">
+        <v>19</v>
+      </c>
+      <c r="J29" s="1">
+        <v>41.476999999999997</v>
+      </c>
+      <c r="K29">
+        <v>-753</v>
+      </c>
+      <c r="L29" s="1">
+        <v>246.26</v>
+      </c>
+      <c r="M29">
+        <v>930.19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>20200107</v>
+      </c>
+      <c r="B30">
+        <v>14</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>2020</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <v>18</v>
+      </c>
+      <c r="I30">
+        <v>19</v>
+      </c>
+      <c r="J30" s="1">
+        <v>41.476999999999997</v>
+      </c>
+      <c r="K30">
+        <v>-752</v>
+      </c>
+      <c r="L30" s="1">
+        <v>249.36</v>
+      </c>
+      <c r="M30">
+        <v>903.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>20200107</v>
+      </c>
+      <c r="B31">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>2020</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <v>18</v>
+      </c>
+      <c r="I31">
+        <v>19</v>
+      </c>
+      <c r="J31" s="1">
+        <v>41.476999999999997</v>
+      </c>
+      <c r="K31">
+        <v>-751</v>
+      </c>
+      <c r="L31" s="1">
+        <v>248.45</v>
+      </c>
+      <c r="M31">
+        <v>879.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>20200107</v>
+      </c>
+      <c r="B32">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>2020</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>10</v>
+      </c>
+      <c r="H32">
+        <v>18</v>
+      </c>
+      <c r="I32">
+        <v>19</v>
+      </c>
+      <c r="J32" s="1">
+        <v>41.476999999999997</v>
+      </c>
+      <c r="K32">
+        <v>-750</v>
+      </c>
+      <c r="L32" s="1">
+        <v>245.53</v>
+      </c>
+      <c r="M32">
+        <v>857.19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>20200107</v>
+      </c>
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>-1141</v>
+      </c>
+      <c r="F33">
+        <v>1276.25</v>
+      </c>
+      <c r="G33">
+        <v>883.59</v>
+      </c>
+      <c r="H33">
+        <v>45.21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>20200107</v>
+      </c>
+      <c r="B34">
+        <v>14</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>-1140</v>
+      </c>
+      <c r="F34">
+        <v>1276.82</v>
+      </c>
+      <c r="G34">
+        <v>940.49</v>
+      </c>
+      <c r="H34">
+        <v>47.72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>20200107</v>
+      </c>
+      <c r="B35">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>-1139</v>
+      </c>
+      <c r="F35">
+        <v>1276.6400000000001</v>
+      </c>
+      <c r="G35">
+        <v>996.56</v>
+      </c>
+      <c r="H35">
+        <v>45.86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>